<commit_message>
Updating with more results
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14120" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="19">
   <si>
     <t>Model + Adjustment</t>
   </si>
@@ -71,12 +71,18 @@
   <si>
     <t>0,25,50,100,200,300,400</t>
   </si>
+  <si>
+    <t>0,25,50,90,150,220,300</t>
+  </si>
+  <si>
+    <t>0,25,50,75,100,150,200</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -112,8 +118,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,6 +151,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -148,7 +167,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -182,23 +201,68 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="11" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -211,8 +275,27 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="87">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -229,6 +312,33 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -245,6 +355,33 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -574,53 +711,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="35.6640625" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="11"/>
-    <col min="8" max="8" width="16.5" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="6"/>
+    <col min="4" max="4" width="21.1640625" style="6" customWidth="1"/>
+    <col min="5" max="7" width="10.83203125" style="6"/>
+    <col min="8" max="8" width="16.5" style="6" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" style="6" customWidth="1"/>
+    <col min="10" max="11" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="68" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" s="15" customFormat="1" ht="68" customHeight="1">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="15" t="s">
         <v>10</v>
       </c>
     </row>
@@ -628,236 +767,256 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="2">
+      <c r="B2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="10">
         <v>3316.922</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="10">
         <v>1.0924400000000001E-2</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="1:11" ht="16">
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="B3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="10">
         <v>3170.0529999999999</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="10">
         <v>2.0748399999999999E-4</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" ht="16">
-      <c r="A4" s="3" t="s">
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+    </row>
+    <row r="4" spans="1:11" s="2" customFormat="1" ht="16">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="4">
+      <c r="B4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="11">
         <v>3116.3620000000001</v>
       </c>
-      <c r="H4" s="4">
+      <c r="G4" s="7"/>
+      <c r="H4" s="11">
         <v>3.5879800000000002E-4</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
     </row>
     <row r="5" spans="1:11" ht="16">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="C5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="10">
         <v>3238.9009999999998</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="10">
         <v>2.9413300000000002E-4</v>
       </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
     </row>
     <row r="6" spans="1:11" ht="16">
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="C6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="10">
         <v>3127.607</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="10">
         <v>1.93743E-3</v>
       </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" s="9" customFormat="1">
-      <c r="E7" s="13"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" spans="1:11" s="5" customFormat="1">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
     </row>
     <row r="8" spans="1:11" ht="16">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="6">
         <v>200</v>
       </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="D8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="10">
         <v>2527.9349999999999</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="12">
         <v>8.0627899999999994E-6</v>
       </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
     </row>
     <row r="9" spans="1:11" ht="16">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="6">
         <v>200</v>
       </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="D9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="10">
         <v>2513.6329999999998</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="10">
         <v>1.41255E-3</v>
       </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" s="3" customFormat="1" ht="16">
-      <c r="A10" s="3" t="s">
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="1:11" s="2" customFormat="1" ht="16">
+      <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="3">
+      <c r="B10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="7">
         <v>200</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="4">
+      <c r="D10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="11">
         <v>2452.7359999999999</v>
       </c>
-      <c r="H10" s="8">
+      <c r="G10" s="7"/>
+      <c r="H10" s="13">
         <v>9.3077500000000008E-6</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:11" s="9" customFormat="1">
-      <c r="E11" s="13"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+    </row>
+    <row r="11" spans="1:11" s="5" customFormat="1">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
     </row>
     <row r="12" spans="1:11" ht="16">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12">
+      <c r="B12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="6">
         <v>400</v>
       </c>
-      <c r="D12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="2">
+      <c r="D12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="10">
         <v>3149.395</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="10">
         <v>5.2703299999999999E-4</v>
       </c>
     </row>
@@ -865,71 +1024,72 @@
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13">
+      <c r="B13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="6">
         <v>400</v>
       </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="2">
+      <c r="D13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="10">
         <v>3072.7890000000002</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="10">
         <v>1.5983E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="3" customFormat="1" ht="16">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:11" s="2" customFormat="1" ht="16">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="3">
+      <c r="B14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="7">
         <v>400</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="4">
+      <c r="D14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="11">
         <v>3027.0250000000001</v>
       </c>
-      <c r="H14" s="4">
+      <c r="G14" s="7"/>
+      <c r="H14" s="11">
         <v>1.67999E-4</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
     </row>
     <row r="15" spans="1:11" ht="16">
       <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="6">
         <v>400</v>
       </c>
-      <c r="D15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="2">
+      <c r="D15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="10">
         <v>3134.7020000000002</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="12">
         <v>8.7468199999999997E-5</v>
       </c>
     </row>
@@ -937,363 +1097,974 @@
       <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="6">
         <v>400</v>
       </c>
-      <c r="D16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="2">
+      <c r="D16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="10">
         <v>3019.6060000000002</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="12">
         <v>6.7430399999999997E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="9" customFormat="1">
-      <c r="E17" s="13"/>
-    </row>
-    <row r="18" spans="1:11" ht="16">
+    <row r="17" spans="1:12" s="5" customFormat="1">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+    </row>
+    <row r="18" spans="1:12" ht="16">
       <c r="A18" t="s">
         <v>11</v>
       </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18">
+      <c r="B18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="6">
         <v>200</v>
       </c>
-      <c r="D18" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="11">
+      <c r="D18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="6">
         <v>20</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="10">
         <v>2512.2310000000002</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="12">
         <v>7.7609100000000002E-5</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="16">
+    <row r="19" spans="1:12" ht="16">
       <c r="A19" t="s">
         <v>12</v>
       </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19">
+      <c r="B19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="6">
         <v>200</v>
       </c>
-      <c r="D19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="11">
+      <c r="D19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="6">
         <v>20</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="10">
         <v>2498.192</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="10">
         <v>1.5484400000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="3" customFormat="1" ht="16">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:12" s="2" customFormat="1" ht="16">
+      <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="3">
+      <c r="B20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="7">
         <v>200</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="12">
+      <c r="D20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="7">
         <v>20</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="11">
         <v>2478.0250000000001</v>
       </c>
-      <c r="H20" s="4">
+      <c r="G20" s="7"/>
+      <c r="H20" s="11">
         <v>5.7347200000000001E-2</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20" s="11">
         <v>3.0717049999999999E-2</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20" s="11">
         <v>1.8783279999999999E-2</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20" s="11">
         <v>5.0232850000000002E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" s="9" customFormat="1">
-      <c r="E21" s="13"/>
-    </row>
-    <row r="22" spans="1:11" ht="16">
+      <c r="L20" s="2">
+        <f>K20 - J20</f>
+        <v>3.1449570000000003E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="5" customFormat="1">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+    </row>
+    <row r="22" spans="1:12" ht="16">
       <c r="A22" t="s">
         <v>11</v>
       </c>
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22">
+      <c r="B22" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="6">
         <v>400</v>
       </c>
-      <c r="D22" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="11">
+      <c r="D22" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="6">
         <v>20</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="10">
         <v>3138.8130000000001</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="10">
         <v>1.8442E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="16">
+    <row r="23" spans="1:12" ht="16">
       <c r="A23" t="s">
         <v>12</v>
       </c>
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23">
+      <c r="B23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="6">
         <v>400</v>
       </c>
-      <c r="D23" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="11">
+      <c r="D23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="6">
         <v>20</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="10">
         <v>3066.5549999999998</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="10">
         <v>3.8243100000000002E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="5" customFormat="1" ht="16">
-      <c r="A24" s="5" t="s">
+    <row r="24" spans="1:12" s="4" customFormat="1" ht="16">
+      <c r="A24" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="5">
+      <c r="B24" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="9">
         <v>400</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="14">
+      <c r="D24" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="9">
         <v>20</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="14">
         <v>3043.3130000000001</v>
       </c>
-      <c r="H24" s="6">
+      <c r="G24" s="9"/>
+      <c r="H24" s="14">
         <v>0.10183300000000001</v>
       </c>
-      <c r="I24" s="6">
+      <c r="I24" s="14">
         <v>3.5248090000000003E-2</v>
       </c>
-      <c r="J24" s="6">
+      <c r="J24" s="14">
         <v>2.1291310000000001E-2</v>
       </c>
-      <c r="K24" s="6">
+      <c r="K24" s="14">
         <v>5.8353740000000001E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" s="3" customFormat="1" ht="16">
-      <c r="A25" s="3" t="s">
+      <c r="L24" s="4">
+        <f>K24 - J24</f>
+        <v>3.706243E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="2" customFormat="1" ht="16">
+      <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="7">
         <v>400</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="12">
+      <c r="D25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="7">
         <v>20</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="11">
         <v>3041.8290000000002</v>
       </c>
-      <c r="H25" s="4">
+      <c r="G25" s="7"/>
+      <c r="H25" s="11">
         <v>3.95731E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" s="9" customFormat="1">
-      <c r="E26" s="13"/>
-    </row>
-    <row r="27" spans="1:11" ht="16">
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+    </row>
+    <row r="26" spans="1:12" s="5" customFormat="1">
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+    </row>
+    <row r="27" spans="1:12" ht="16">
       <c r="A27" t="s">
         <v>11</v>
       </c>
-      <c r="B27" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27">
+      <c r="B27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="6">
         <v>400</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="2">
+      <c r="E27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="10">
         <v>1015.191</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="16">
+    <row r="28" spans="1:12" ht="16">
       <c r="A28" t="s">
         <v>12</v>
       </c>
-      <c r="B28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28">
+      <c r="B28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="6">
         <v>400</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="2">
-        <v>941.26840000000004</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="A29" s="5" t="s">
+      <c r="E28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="10">
+        <v>942.62</v>
+      </c>
+      <c r="G28" s="10">
+        <v>6.0600000000000003E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="2" customFormat="1" ht="16">
+      <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B29" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29">
+      <c r="B29" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="7">
         <v>400</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="5" t="s">
+      <c r="E29" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="11">
+        <v>932.85410000000002</v>
+      </c>
+      <c r="G29" s="11">
+        <v>0.65581</v>
+      </c>
+      <c r="H29" s="7"/>
+      <c r="I29" s="11">
+        <v>1.9591549999999999E-2</v>
+      </c>
+      <c r="J29" s="11">
+        <v>1.2209739000000001E-2</v>
+      </c>
+      <c r="K29" s="11">
+        <v>3.1436279999999997E-2</v>
+      </c>
+      <c r="L29" s="2">
+        <f>K29 - J29</f>
+        <v>1.9226540999999996E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="16">
+      <c r="A30" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="6">
         <v>400</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E30" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" s="9" customFormat="1">
-      <c r="E31" s="13"/>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="E30" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="10">
+        <v>0.44539000000000001</v>
+      </c>
+      <c r="G30" s="10">
+        <v>0.44539000000000001</v>
+      </c>
+      <c r="I30" s="10">
+        <v>1.749231E-2</v>
+      </c>
+      <c r="J30" s="10">
+        <v>1.120352E-2</v>
+      </c>
+      <c r="K30" s="10">
+        <v>2.7311160000000001E-2</v>
+      </c>
+      <c r="L30" s="4">
+        <f>K30 - J30</f>
+        <v>1.6107639999999999E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="5" customFormat="1">
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+    </row>
+    <row r="32" spans="1:12" ht="16">
       <c r="A32" t="s">
         <v>11</v>
       </c>
-      <c r="B32" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32">
+      <c r="B32" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="6">
         <v>400</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E32" s="11">
+      <c r="E32" s="6">
         <v>20</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" s="10">
+        <v>1011.293</v>
+      </c>
+      <c r="G32" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="16">
       <c r="A33" t="s">
         <v>12</v>
       </c>
-      <c r="B33" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33">
+      <c r="B33" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="6">
         <v>400</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E33" s="11">
+      <c r="E33" s="6">
         <v>20</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="5" t="s">
+      <c r="F33" s="10">
+        <v>944.1318</v>
+      </c>
+      <c r="G33" s="10">
+        <v>3.8597000000000002E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="16">
+      <c r="A34" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B34" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34">
+      <c r="B34" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="6">
         <v>400</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E34" s="11">
+      <c r="E34" s="6">
         <v>20</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="5" t="s">
+      <c r="F34" s="10">
+        <v>932.40869999999995</v>
+      </c>
+      <c r="G34" s="10">
+        <v>0.92452999999999996</v>
+      </c>
+      <c r="I34" s="10">
+        <v>2.0305420000000001E-2</v>
+      </c>
+      <c r="J34" s="10">
+        <v>1.258895E-2</v>
+      </c>
+      <c r="K34" s="10">
+        <v>3.275173E-2</v>
+      </c>
+      <c r="L34" s="4">
+        <f>K34 - J34</f>
+        <v>2.0162779999999998E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" s="2" customFormat="1" ht="16">
+      <c r="A35" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="7">
         <v>400</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E35" s="11">
+      <c r="E35" s="7">
         <v>20</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" s="9" customFormat="1">
-      <c r="E36" s="13"/>
+      <c r="F35" s="11">
+        <v>930.2722</v>
+      </c>
+      <c r="G35" s="11">
+        <v>0.75787000000000004</v>
+      </c>
+      <c r="H35" s="7"/>
+      <c r="I35" s="11">
+        <v>1.7769279999999998E-2</v>
+      </c>
+      <c r="J35" s="11">
+        <v>1.1392546999999999E-2</v>
+      </c>
+      <c r="K35" s="11">
+        <v>2.7715239999999999E-2</v>
+      </c>
+      <c r="L35" s="2">
+        <f>K35 - J35</f>
+        <v>1.6322692999999999E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" s="5" customFormat="1">
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+    </row>
+    <row r="37" spans="1:12" ht="16">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="6">
+        <v>300</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37" s="1">
+        <v>954.52970000000005</v>
+      </c>
+      <c r="G37" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="16">
+      <c r="A38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="6">
+        <v>300</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F38" s="1">
+        <v>916.94349999999997</v>
+      </c>
+      <c r="G38" s="1">
+        <v>8.7036000000000002E-2</v>
+      </c>
+      <c r="I38" s="1">
+        <v>1.7405779999999999E-2</v>
+      </c>
+      <c r="J38" s="1">
+        <v>1.1159486999999999E-2</v>
+      </c>
+      <c r="K38" s="1">
+        <v>2.71483E-2</v>
+      </c>
+      <c r="L38" s="4">
+        <f>K38 - J38</f>
+        <v>1.5988813000000001E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" s="2" customFormat="1" ht="16">
+      <c r="A39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="7">
+        <v>300</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" s="3">
+        <v>910.81659999999999</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0.83374999999999999</v>
+      </c>
+      <c r="H39" s="7"/>
+      <c r="I39" s="3">
+        <v>2.0097159999999999E-2</v>
+      </c>
+      <c r="J39" s="3">
+        <v>1.2265219000000001E-2</v>
+      </c>
+      <c r="K39" s="3">
+        <v>3.2930180000000003E-2</v>
+      </c>
+      <c r="L39" s="2">
+        <f>K39 - J39</f>
+        <v>2.0664961000000003E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="16">
+      <c r="A40" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="6">
+        <v>300</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" s="1">
+        <v>911.04280000000006</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0.64603999999999995</v>
+      </c>
+      <c r="I40" s="1">
+        <v>1.8222599999999999E-2</v>
+      </c>
+      <c r="J40" s="1">
+        <v>1.13641E-2</v>
+      </c>
+      <c r="K40" s="1">
+        <v>2.9220349999999999E-2</v>
+      </c>
+      <c r="L40" s="4">
+        <f>K40 - J40</f>
+        <v>1.7856249999999997E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="5" customFormat="1">
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+    </row>
+    <row r="42" spans="1:12" ht="16">
+      <c r="A42" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="6">
+        <v>300</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="6">
+        <v>20</v>
+      </c>
+      <c r="F42" s="1">
+        <v>953.8261</v>
+      </c>
+      <c r="G42" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="16">
+      <c r="A43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="6">
+        <v>300</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="6">
+        <v>20</v>
+      </c>
+      <c r="F43" s="1">
+        <v>909.78930000000003</v>
+      </c>
+      <c r="G43" s="1">
+        <v>9.0878E-2</v>
+      </c>
+      <c r="I43" s="1">
+        <v>1.7670979999999999E-2</v>
+      </c>
+      <c r="J43" s="1">
+        <v>1.1373477999999999E-2</v>
+      </c>
+      <c r="K43" s="1">
+        <v>2.7455429999999999E-2</v>
+      </c>
+      <c r="L43" s="4">
+        <f>K43 - J43</f>
+        <v>1.6081952E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" s="2" customFormat="1" ht="16">
+      <c r="A44" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="7">
+        <v>300</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E44" s="7">
+        <v>20</v>
+      </c>
+      <c r="F44" s="3">
+        <v>903.36479999999995</v>
+      </c>
+      <c r="G44" s="3">
+        <v>0.92720999999999998</v>
+      </c>
+      <c r="H44" s="7"/>
+      <c r="I44" s="3">
+        <v>2.0958210000000001E-2</v>
+      </c>
+      <c r="J44" s="3">
+        <v>1.2757271000000001E-2</v>
+      </c>
+      <c r="K44" s="3">
+        <v>3.4431059999999999E-2</v>
+      </c>
+      <c r="L44" s="2">
+        <f>K44 - J44</f>
+        <v>2.1673788999999999E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="16">
+      <c r="A45" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="6">
+        <v>300</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" s="6">
+        <v>20</v>
+      </c>
+      <c r="F45" s="1">
+        <v>904.62419999999997</v>
+      </c>
+      <c r="G45" s="1">
+        <v>0.7853</v>
+      </c>
+      <c r="I45" s="1">
+        <v>1.939861E-2</v>
+      </c>
+      <c r="J45" s="1">
+        <v>1.2027919999999999E-2</v>
+      </c>
+      <c r="K45" s="1">
+        <v>3.1286040000000001E-2</v>
+      </c>
+      <c r="L45" s="4">
+        <f>K45 - J45</f>
+        <v>1.9258120000000004E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" s="5" customFormat="1">
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+    </row>
+    <row r="47" spans="1:12" ht="16">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="6">
+        <v>200</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" s="1">
+        <v>834.05399999999997</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0.10629</v>
+      </c>
+      <c r="I47" s="1">
+        <v>1.6649959999999998E-2</v>
+      </c>
+      <c r="J47" s="1">
+        <v>1.0716079999999999E-2</v>
+      </c>
+      <c r="K47" s="1">
+        <v>2.5869630000000001E-2</v>
+      </c>
+      <c r="L47" s="4">
+        <f>K47 - J47</f>
+        <v>1.5153550000000002E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" s="2" customFormat="1" ht="16">
+      <c r="A48" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="7">
+        <v>200</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48" s="3">
+        <v>830.16930000000002</v>
+      </c>
+      <c r="G48" s="3">
+        <v>0.54693000000000003</v>
+      </c>
+      <c r="H48" s="7"/>
+      <c r="I48" s="3">
+        <v>1.981103E-2</v>
+      </c>
+      <c r="J48" s="3">
+        <v>1.1904585000000001E-2</v>
+      </c>
+      <c r="K48" s="3">
+        <v>3.2968560000000001E-2</v>
+      </c>
+      <c r="L48" s="2">
+        <f>K48 - J48</f>
+        <v>2.1063974999999999E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" s="5" customFormat="1">
+      <c r="A49" s="16"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+    </row>
+    <row r="50" spans="1:12" ht="16">
+      <c r="A50" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" s="6">
+        <v>200</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E50" s="6">
+        <v>20</v>
+      </c>
+      <c r="F50" s="1">
+        <v>838.15440000000001</v>
+      </c>
+      <c r="G50" s="1">
+        <v>4.9900999999999999E-3</v>
+      </c>
+      <c r="I50" s="1">
+        <v>1.68075E-2</v>
+      </c>
+      <c r="J50" s="1">
+        <v>1.0802045E-2</v>
+      </c>
+      <c r="K50" s="1">
+        <v>2.6151710000000002E-2</v>
+      </c>
+      <c r="L50" s="4">
+        <f>K50 - J50</f>
+        <v>1.5349665000000002E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" s="2" customFormat="1" ht="16">
+      <c r="A51" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" s="7">
+        <v>200</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E51" s="7">
+        <v>20</v>
+      </c>
+      <c r="F51" s="3">
+        <v>832.35260000000005</v>
+      </c>
+      <c r="G51" s="3">
+        <v>8.2095000000000001E-2</v>
+      </c>
+      <c r="H51" s="7"/>
+      <c r="I51" s="3">
+        <v>2.1046780000000001E-2</v>
+      </c>
+      <c r="J51" s="3">
+        <v>1.2430237E-2</v>
+      </c>
+      <c r="K51" s="3">
+        <v>3.5636260000000003E-2</v>
+      </c>
+      <c r="L51" s="2">
+        <f>K51 - J51</f>
+        <v>2.3206023000000003E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" s="5" customFormat="1">
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Starting to choose model
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamese.richardson/Projects/msc/hares/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569C71F7-34B8-F94E-A73A-B3C9EFD453A0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="22">
   <si>
     <t>Model + Adjustment</t>
   </si>
@@ -77,12 +83,21 @@
   <si>
     <t>0,25,50,75,100,150,200</t>
   </si>
+  <si>
+    <t>0,25,50,90,150,220,300,400</t>
+  </si>
+  <si>
+    <t>Hazard rate + Cos</t>
+  </si>
+  <si>
+    <t>Hazard rate + Poly</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -124,6 +139,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Monaco"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -256,7 +277,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -294,6 +315,8 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="87">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -386,6 +409,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -710,25 +741,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="L44" sqref="L44"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A12" zoomScale="113" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.6640625" customWidth="1"/>
     <col min="2" max="3" width="10.83203125" style="6"/>
-    <col min="4" max="4" width="21.1640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="31" style="6" customWidth="1"/>
     <col min="5" max="7" width="10.83203125" style="6"/>
     <col min="8" max="8" width="16.5" style="6" customWidth="1"/>
     <col min="9" max="9" width="16.33203125" style="6" customWidth="1"/>
     <col min="10" max="11" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="15" customFormat="1" ht="68" customHeight="1">
+    <row r="1" spans="1:11" s="15" customFormat="1" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -763,7 +794,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -789,7 +820,7 @@
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
     </row>
-    <row r="3" spans="1:11" ht="16">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -815,7 +846,7 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" ht="16">
+    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -842,7 +873,7 @@
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
     </row>
-    <row r="5" spans="1:11" ht="16">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -868,7 +899,7 @@
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" ht="16">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -894,7 +925,7 @@
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" s="5" customFormat="1">
+    <row r="7" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -906,7 +937,7 @@
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="1:11" ht="16">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -932,7 +963,7 @@
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" ht="16">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -958,7 +989,7 @@
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" s="2" customFormat="1" ht="16">
+    <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -985,7 +1016,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
     </row>
-    <row r="11" spans="1:11" s="5" customFormat="1">
+    <row r="11" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -997,7 +1028,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" ht="16">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1020,7 +1051,7 @@
         <v>5.2703299999999999E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="16">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1043,7 +1074,7 @@
         <v>1.5983E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="2" customFormat="1" ht="16">
+    <row r="14" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1070,7 +1101,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
     </row>
-    <row r="15" spans="1:11" ht="16">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1093,7 +1124,7 @@
         <v>8.7468199999999997E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="16">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1116,7 +1147,7 @@
         <v>6.7430399999999997E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="5" customFormat="1">
+    <row r="17" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -1128,7 +1159,7 @@
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
     </row>
-    <row r="18" spans="1:12" ht="16">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1151,7 +1182,7 @@
         <v>7.7609100000000002E-5</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="16">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1174,7 +1205,7 @@
         <v>1.5484400000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="2" customFormat="1" ht="16">
+    <row r="20" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
@@ -1211,7 +1242,7 @@
         <v>3.1449570000000003E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="5" customFormat="1">
+    <row r="21" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -1223,7 +1254,7 @@
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
     </row>
-    <row r="22" spans="1:12" ht="16">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1246,7 +1277,7 @@
         <v>1.8442E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="16">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1269,7 +1300,7 @@
         <v>3.8243100000000002E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="4" customFormat="1" ht="16">
+    <row r="24" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>13</v>
       </c>
@@ -1306,7 +1337,7 @@
         <v>3.706243E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="2" customFormat="1" ht="16">
+    <row r="25" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
@@ -1333,7 +1364,7 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:12" s="5" customFormat="1">
+    <row r="26" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -1345,7 +1376,7 @@
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
     </row>
-    <row r="27" spans="1:12" ht="16">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -1368,7 +1399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="16">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -1391,7 +1422,7 @@
         <v>6.0600000000000003E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="2" customFormat="1" ht="16">
+    <row r="29" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
@@ -1428,7 +1459,7 @@
         <v>1.9226540999999996E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="16">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>13</v>
       </c>
@@ -1464,7 +1495,7 @@
         <v>1.6107639999999999E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="5" customFormat="1">
+    <row r="31" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -1476,7 +1507,7 @@
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
     </row>
-    <row r="32" spans="1:12" ht="16">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -1499,7 +1530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="16">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -1522,7 +1553,7 @@
         <v>3.8597000000000002E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="16">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>13</v>
       </c>
@@ -1558,7 +1589,7 @@
         <v>2.0162779999999998E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="2" customFormat="1" ht="16">
+    <row r="35" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>13</v>
       </c>
@@ -1595,7 +1626,7 @@
         <v>1.6322692999999999E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="5" customFormat="1">
+    <row r="36" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -1607,7 +1638,7 @@
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
     </row>
-    <row r="37" spans="1:12" ht="16">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -1630,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="16">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -1666,7 +1697,7 @@
         <v>1.5988813000000001E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="2" customFormat="1" ht="16">
+    <row r="39" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>13</v>
       </c>
@@ -1703,7 +1734,7 @@
         <v>2.0664961000000003E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="16">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>13</v>
       </c>
@@ -1739,7 +1770,7 @@
         <v>1.7856249999999997E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="5" customFormat="1">
+    <row r="41" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
@@ -1751,7 +1782,7 @@
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
     </row>
-    <row r="42" spans="1:12" ht="16">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -1774,7 +1805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="16">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -1810,7 +1841,7 @@
         <v>1.6081952E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="2" customFormat="1" ht="16">
+    <row r="44" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>13</v>
       </c>
@@ -1847,7 +1878,7 @@
         <v>2.1673788999999999E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="16">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>13</v>
       </c>
@@ -1883,7 +1914,7 @@
         <v>1.9258120000000004E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:12" s="5" customFormat="1">
+    <row r="46" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
@@ -1895,7 +1926,7 @@
       <c r="J46" s="8"/>
       <c r="K46" s="8"/>
     </row>
-    <row r="47" spans="1:12" ht="16">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -1931,7 +1962,7 @@
         <v>1.5153550000000002E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="2" customFormat="1" ht="16">
+    <row r="48" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>13</v>
       </c>
@@ -1968,7 +1999,7 @@
         <v>2.1063974999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="5" customFormat="1">
+    <row r="49" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="16"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
@@ -1981,7 +2012,7 @@
       <c r="J49" s="8"/>
       <c r="K49" s="8"/>
     </row>
-    <row r="50" spans="1:12" ht="16">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -2017,7 +2048,7 @@
         <v>1.5349665000000002E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:12" s="2" customFormat="1" ht="16">
+    <row r="51" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>13</v>
       </c>
@@ -2054,7 +2085,7 @@
         <v>2.3206023000000003E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:12" s="5" customFormat="1">
+    <row r="52" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
@@ -2066,6 +2097,187 @@
       <c r="J52" s="8"/>
       <c r="K52" s="8"/>
     </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="6">
+        <v>400</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F53" s="17">
+        <v>1013.923</v>
+      </c>
+      <c r="G53" s="17">
+        <v>2.8326E-2</v>
+      </c>
+      <c r="I53" s="17">
+        <v>1.6755450000000002E-2</v>
+      </c>
+      <c r="J53" s="17">
+        <v>1.0740981E-2</v>
+      </c>
+      <c r="K53" s="17">
+        <v>2.6137750000000001E-2</v>
+      </c>
+      <c r="L53" s="4">
+        <f>K53 - J53</f>
+        <v>1.5396769000000001E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" s="6">
+        <v>400</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F54" s="17">
+        <v>1005.018</v>
+      </c>
+      <c r="G54" s="17">
+        <v>0.75468000000000002</v>
+      </c>
+      <c r="I54" s="17">
+        <v>1.9822159999999998E-2</v>
+      </c>
+      <c r="J54" s="17">
+        <v>1.2295250000000001E-2</v>
+      </c>
+      <c r="K54" s="17">
+        <v>3.195688E-2</v>
+      </c>
+      <c r="L54" s="4">
+        <f>K54 - J54</f>
+        <v>1.9661629999999999E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C55" s="7">
+        <v>400</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F55" s="18">
+        <v>1003.018</v>
+      </c>
+      <c r="G55" s="18">
+        <v>0.59157999999999999</v>
+      </c>
+      <c r="H55" s="7"/>
+      <c r="I55" s="18">
+        <v>1.7540469999999999E-2</v>
+      </c>
+      <c r="J55" s="18">
+        <v>1.1209897999999999E-2</v>
+      </c>
+      <c r="K55" s="18">
+        <v>2.7446109999999999E-2</v>
+      </c>
+      <c r="L55" s="2">
+        <f>K55 - J55</f>
+        <v>1.6236212E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="6">
+        <v>400</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F56" s="17">
+        <v>1003.018</v>
+      </c>
+      <c r="G56" s="17">
+        <v>0.59157999999999999</v>
+      </c>
+      <c r="I56" s="17">
+        <v>1.7540469999999999E-2</v>
+      </c>
+      <c r="J56" s="17">
+        <v>1.1209897999999999E-2</v>
+      </c>
+      <c r="K56" s="17">
+        <v>2.7446109999999999E-2</v>
+      </c>
+      <c r="L56" s="4">
+        <f>K56 - J56</f>
+        <v>1.6236212E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>21</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C57" s="6">
+        <v>400</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F57" s="17">
+        <v>1003.018</v>
+      </c>
+      <c r="G57" s="17">
+        <v>0.59157999999999999</v>
+      </c>
+      <c r="I57" s="17">
+        <v>1.7540469999999999E-2</v>
+      </c>
+      <c r="J57" s="17">
+        <v>1.1209897999999999E-2</v>
+      </c>
+      <c r="K57" s="17">
+        <v>2.7446109999999999E-2</v>
+      </c>
+      <c r="L57" s="4">
+        <f>K57 - J57</f>
+        <v>1.6236212E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Updating report and results
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamese.richardson/Projects/msc/hares/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569C71F7-34B8-F94E-A73A-B3C9EFD453A0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D802A114-4BAC-6648-B2F2-4F3DAEA349C1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -744,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A12" zoomScale="113" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A23" zoomScale="113" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updating report with all data and graphs as evidence
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10523"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamese.richardson/Projects/msc/hares/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamese.richardson/Projects/Masters/msc-distance-hares/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D802A114-4BAC-6648-B2F2-4F3DAEA349C1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C13F530-450F-7449-B3B9-DCACAFB446FE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="17740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="22">
   <si>
     <t>Model + Adjustment</t>
   </si>
@@ -97,7 +97,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -146,8 +146,14 @@
       <name val="Monaco"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Monaco"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,6 +184,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -277,7 +289,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -317,6 +329,19 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="87">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -742,24 +767,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A23" zoomScale="113" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1"/>
-    <col min="2" max="3" width="10.83203125" style="6"/>
-    <col min="4" max="4" width="31" style="6" customWidth="1"/>
-    <col min="5" max="7" width="10.83203125" style="6"/>
-    <col min="8" max="8" width="16.5" style="6" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" style="6" customWidth="1"/>
-    <col min="10" max="11" width="10.83203125" style="6"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="6" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="15" style="6" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" style="6" hidden="1" customWidth="1"/>
+    <col min="10" max="11" width="0" style="6" hidden="1" customWidth="1"/>
+    <col min="12" max="14" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="15" customFormat="1" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="15" customFormat="1" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -793,8 +821,17 @@
       <c r="K1" s="15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -820,7 +857,7 @@
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -846,7 +883,7 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -873,7 +910,7 @@
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -899,7 +936,7 @@
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -925,7 +962,7 @@
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -937,7 +974,7 @@
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -963,7 +1000,7 @@
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -989,7 +1026,7 @@
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1016,7 +1053,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
     </row>
-    <row r="11" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -1028,7 +1065,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1051,7 +1088,7 @@
         <v>5.2703299999999999E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1074,7 +1111,7 @@
         <v>1.5983E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1101,7 +1138,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1124,7 +1161,7 @@
         <v>8.7468199999999997E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1147,7 +1184,7 @@
         <v>6.7430399999999997E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -1159,7 +1196,7 @@
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1182,7 +1219,7 @@
         <v>7.7609100000000002E-5</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1205,7 +1242,7 @@
         <v>1.5484400000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
@@ -1237,12 +1274,20 @@
       <c r="K20" s="11">
         <v>5.0232850000000002E-2</v>
       </c>
-      <c r="L20" s="2">
-        <f>K20 - J20</f>
-        <v>3.1449570000000003E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L20" s="19">
+        <f>I20 * 1000</f>
+        <v>30.71705</v>
+      </c>
+      <c r="M20" s="19">
+        <f t="shared" ref="M20:N20" si="0">J20 * 1000</f>
+        <v>18.783279999999998</v>
+      </c>
+      <c r="N20" s="19">
+        <f t="shared" si="0"/>
+        <v>50.232849999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -1254,7 +1299,7 @@
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1277,7 +1322,7 @@
         <v>1.8442E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1300,7 +1345,7 @@
         <v>3.8243100000000002E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>13</v>
       </c>
@@ -1332,12 +1377,20 @@
       <c r="K24" s="14">
         <v>5.8353740000000001E-2</v>
       </c>
-      <c r="L24" s="4">
-        <f>K24 - J24</f>
-        <v>3.706243E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L24" s="20">
+        <f>I24 * 1000</f>
+        <v>35.248090000000005</v>
+      </c>
+      <c r="M24" s="20">
+        <f t="shared" ref="M24" si="1">J24 * 1000</f>
+        <v>21.291309999999999</v>
+      </c>
+      <c r="N24" s="20">
+        <f t="shared" ref="N24" si="2">K24 * 1000</f>
+        <v>58.353740000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
@@ -1364,7 +1417,7 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -1376,7 +1429,7 @@
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -1395,11 +1448,11 @@
       <c r="F27" s="10">
         <v>1015.191</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G27" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -1422,44 +1475,52 @@
         <v>6.0600000000000003E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="7">
+      <c r="B29" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="22">
         <v>400</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="11">
+      <c r="E29" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="23">
         <v>932.85410000000002</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G29" s="23">
         <v>0.65581</v>
       </c>
-      <c r="H29" s="7"/>
-      <c r="I29" s="11">
+      <c r="H29" s="22"/>
+      <c r="I29" s="23">
         <v>1.9591549999999999E-2</v>
       </c>
-      <c r="J29" s="11">
+      <c r="J29" s="23">
         <v>1.2209739000000001E-2</v>
       </c>
-      <c r="K29" s="11">
+      <c r="K29" s="23">
         <v>3.1436279999999997E-2</v>
       </c>
-      <c r="L29" s="2">
-        <f>K29 - J29</f>
-        <v>1.9226540999999996E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L29" s="24">
+        <f>I29 * 1000</f>
+        <v>19.591549999999998</v>
+      </c>
+      <c r="M29" s="24">
+        <f t="shared" ref="M29:M30" si="3">J29 * 1000</f>
+        <v>12.209739000000001</v>
+      </c>
+      <c r="N29" s="24">
+        <f t="shared" ref="N29:N30" si="4">K29 * 1000</f>
+        <v>31.436279999999996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>13</v>
       </c>
@@ -1490,12 +1551,20 @@
       <c r="K30" s="10">
         <v>2.7311160000000001E-2</v>
       </c>
-      <c r="L30" s="4">
-        <f>K30 - J30</f>
-        <v>1.6107639999999999E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L30" s="20">
+        <f>I30 * 1000</f>
+        <v>17.49231</v>
+      </c>
+      <c r="M30" s="20">
+        <f t="shared" si="3"/>
+        <v>11.203519999999999</v>
+      </c>
+      <c r="N30" s="20">
+        <f t="shared" si="4"/>
+        <v>27.311160000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -1507,7 +1576,7 @@
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -1526,11 +1595,11 @@
       <c r="F32" s="10">
         <v>1011.293</v>
       </c>
-      <c r="G32" s="6">
+      <c r="G32" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -1553,7 +1622,7 @@
         <v>3.8597000000000002E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>13</v>
       </c>
@@ -1584,12 +1653,20 @@
       <c r="K34" s="10">
         <v>3.275173E-2</v>
       </c>
-      <c r="L34" s="4">
-        <f>K34 - J34</f>
-        <v>2.0162779999999998E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L34" s="20">
+        <f>I34 * 1000</f>
+        <v>20.305420000000002</v>
+      </c>
+      <c r="M34" s="20">
+        <f t="shared" ref="M34:M35" si="5">J34 * 1000</f>
+        <v>12.588950000000001</v>
+      </c>
+      <c r="N34" s="20">
+        <f t="shared" ref="N34:N35" si="6">K34 * 1000</f>
+        <v>32.751730000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>13</v>
       </c>
@@ -1621,12 +1698,20 @@
       <c r="K35" s="11">
         <v>2.7715239999999999E-2</v>
       </c>
-      <c r="L35" s="2">
-        <f>K35 - J35</f>
-        <v>1.6322692999999999E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L35" s="19">
+        <f>I35 * 1000</f>
+        <v>17.769279999999998</v>
+      </c>
+      <c r="M35" s="19">
+        <f t="shared" si="5"/>
+        <v>11.392546999999999</v>
+      </c>
+      <c r="N35" s="19">
+        <f t="shared" si="6"/>
+        <v>27.715239999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -1638,7 +1723,7 @@
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -1661,7 +1746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -1692,12 +1777,20 @@
       <c r="K38" s="1">
         <v>2.71483E-2</v>
       </c>
-      <c r="L38" s="4">
-        <f>K38 - J38</f>
-        <v>1.5988813000000001E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L38" s="20">
+        <f>I38 * 1000</f>
+        <v>17.40578</v>
+      </c>
+      <c r="M38" s="20">
+        <f t="shared" ref="M38:M39" si="7">J38 * 1000</f>
+        <v>11.159486999999999</v>
+      </c>
+      <c r="N38" s="20">
+        <f t="shared" ref="N38:N39" si="8">K38 * 1000</f>
+        <v>27.148299999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>13</v>
       </c>
@@ -1729,12 +1822,20 @@
       <c r="K39" s="3">
         <v>3.2930180000000003E-2</v>
       </c>
-      <c r="L39" s="2">
-        <f>K39 - J39</f>
-        <v>2.0664961000000003E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L39" s="19">
+        <f>I39 * 1000</f>
+        <v>20.097159999999999</v>
+      </c>
+      <c r="M39" s="19">
+        <f t="shared" si="7"/>
+        <v>12.265219</v>
+      </c>
+      <c r="N39" s="19">
+        <f t="shared" si="8"/>
+        <v>32.93018</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>13</v>
       </c>
@@ -1765,12 +1866,20 @@
       <c r="K40" s="1">
         <v>2.9220349999999999E-2</v>
       </c>
-      <c r="L40" s="4">
-        <f>K40 - J40</f>
-        <v>1.7856249999999997E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L40" s="20">
+        <f>I40 * 1000</f>
+        <v>18.2226</v>
+      </c>
+      <c r="M40" s="20">
+        <f t="shared" ref="M40" si="9">J40 * 1000</f>
+        <v>11.364100000000001</v>
+      </c>
+      <c r="N40" s="20">
+        <f t="shared" ref="N40" si="10">K40 * 1000</f>
+        <v>29.22035</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
@@ -1782,7 +1891,7 @@
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -1805,7 +1914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -1836,12 +1945,20 @@
       <c r="K43" s="1">
         <v>2.7455429999999999E-2</v>
       </c>
-      <c r="L43" s="4">
-        <f>K43 - J43</f>
-        <v>1.6081952E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L43" s="20">
+        <f>I43 * 1000</f>
+        <v>17.67098</v>
+      </c>
+      <c r="M43" s="20">
+        <f t="shared" ref="M43:M44" si="11">J43 * 1000</f>
+        <v>11.373477999999999</v>
+      </c>
+      <c r="N43" s="20">
+        <f t="shared" ref="N43:N44" si="12">K43 * 1000</f>
+        <v>27.45543</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>13</v>
       </c>
@@ -1873,12 +1990,20 @@
       <c r="K44" s="3">
         <v>3.4431059999999999E-2</v>
       </c>
-      <c r="L44" s="2">
-        <f>K44 - J44</f>
-        <v>2.1673788999999999E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L44" s="19">
+        <f>I44 * 1000</f>
+        <v>20.958210000000001</v>
+      </c>
+      <c r="M44" s="19">
+        <f t="shared" si="11"/>
+        <v>12.757271000000001</v>
+      </c>
+      <c r="N44" s="19">
+        <f t="shared" si="12"/>
+        <v>34.431060000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>13</v>
       </c>
@@ -1909,12 +2034,20 @@
       <c r="K45" s="1">
         <v>3.1286040000000001E-2</v>
       </c>
-      <c r="L45" s="4">
-        <f>K45 - J45</f>
-        <v>1.9258120000000004E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L45" s="20">
+        <f>I45 * 1000</f>
+        <v>19.398610000000001</v>
+      </c>
+      <c r="M45" s="20">
+        <f t="shared" ref="M45" si="13">J45 * 1000</f>
+        <v>12.02792</v>
+      </c>
+      <c r="N45" s="20">
+        <f t="shared" ref="N45" si="14">K45 * 1000</f>
+        <v>31.28604</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
@@ -1926,7 +2059,7 @@
       <c r="J46" s="8"/>
       <c r="K46" s="8"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -1957,12 +2090,20 @@
       <c r="K47" s="1">
         <v>2.5869630000000001E-2</v>
       </c>
-      <c r="L47" s="4">
-        <f>K47 - J47</f>
-        <v>1.5153550000000002E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L47" s="20">
+        <f>I47 * 1000</f>
+        <v>16.64996</v>
+      </c>
+      <c r="M47" s="20">
+        <f t="shared" ref="M47" si="15">J47 * 1000</f>
+        <v>10.71608</v>
+      </c>
+      <c r="N47" s="20">
+        <f t="shared" ref="N47" si="16">K47 * 1000</f>
+        <v>25.869630000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>13</v>
       </c>
@@ -1994,12 +2135,20 @@
       <c r="K48" s="3">
         <v>3.2968560000000001E-2</v>
       </c>
-      <c r="L48" s="2">
-        <f>K48 - J48</f>
-        <v>2.1063974999999999E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L48" s="19">
+        <f>I48 * 1000</f>
+        <v>19.811029999999999</v>
+      </c>
+      <c r="M48" s="19">
+        <f t="shared" ref="M48" si="17">J48 * 1000</f>
+        <v>11.904585000000001</v>
+      </c>
+      <c r="N48" s="19">
+        <f t="shared" ref="N48" si="18">K48 * 1000</f>
+        <v>32.968560000000004</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="16"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
@@ -2012,7 +2161,7 @@
       <c r="J49" s="8"/>
       <c r="K49" s="8"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -2043,12 +2192,20 @@
       <c r="K50" s="1">
         <v>2.6151710000000002E-2</v>
       </c>
-      <c r="L50" s="4">
-        <f>K50 - J50</f>
-        <v>1.5349665000000002E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L50" s="20">
+        <f>I50 * 1000</f>
+        <v>16.807500000000001</v>
+      </c>
+      <c r="M50" s="20">
+        <f t="shared" ref="M50" si="19">J50 * 1000</f>
+        <v>10.802045</v>
+      </c>
+      <c r="N50" s="20">
+        <f t="shared" ref="N50" si="20">K50 * 1000</f>
+        <v>26.151710000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>13</v>
       </c>
@@ -2080,12 +2237,20 @@
       <c r="K51" s="3">
         <v>3.5636260000000003E-2</v>
       </c>
-      <c r="L51" s="2">
-        <f>K51 - J51</f>
-        <v>2.3206023000000003E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L51" s="19">
+        <f>I51 * 1000</f>
+        <v>21.046780000000002</v>
+      </c>
+      <c r="M51" s="19">
+        <f t="shared" ref="M51" si="21">J51 * 1000</f>
+        <v>12.430237</v>
+      </c>
+      <c r="N51" s="19">
+        <f t="shared" ref="N51" si="22">K51 * 1000</f>
+        <v>35.63626</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
@@ -2097,7 +2262,7 @@
       <c r="J52" s="8"/>
       <c r="K52" s="8"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -2128,12 +2293,20 @@
       <c r="K53" s="17">
         <v>2.6137750000000001E-2</v>
       </c>
-      <c r="L53" s="4">
-        <f>K53 - J53</f>
-        <v>1.5396769000000001E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L53" s="20">
+        <f>I53 * 1000</f>
+        <v>16.755450000000003</v>
+      </c>
+      <c r="M53" s="20">
+        <f t="shared" ref="M53:M54" si="23">J53 * 1000</f>
+        <v>10.740981</v>
+      </c>
+      <c r="N53" s="20">
+        <f t="shared" ref="N53:N54" si="24">K53 * 1000</f>
+        <v>26.13775</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>13</v>
       </c>
@@ -2164,12 +2337,20 @@
       <c r="K54" s="17">
         <v>3.195688E-2</v>
       </c>
-      <c r="L54" s="4">
-        <f>K54 - J54</f>
-        <v>1.9661629999999999E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L54" s="20">
+        <f>I54 * 1000</f>
+        <v>19.822159999999997</v>
+      </c>
+      <c r="M54" s="20">
+        <f t="shared" si="23"/>
+        <v>12.295250000000001</v>
+      </c>
+      <c r="N54" s="20">
+        <f t="shared" si="24"/>
+        <v>31.956880000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>13</v>
       </c>
@@ -2201,12 +2382,20 @@
       <c r="K55" s="18">
         <v>2.7446109999999999E-2</v>
       </c>
-      <c r="L55" s="2">
-        <f>K55 - J55</f>
-        <v>1.6236212E-2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L55" s="19">
+        <f>I55 * 1000</f>
+        <v>17.540469999999999</v>
+      </c>
+      <c r="M55" s="19">
+        <f t="shared" ref="M55:M57" si="25">J55 * 1000</f>
+        <v>11.209897999999999</v>
+      </c>
+      <c r="N55" s="19">
+        <f t="shared" ref="N55:N57" si="26">K55 * 1000</f>
+        <v>27.446110000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>20</v>
       </c>
@@ -2237,12 +2426,20 @@
       <c r="K56" s="17">
         <v>2.7446109999999999E-2</v>
       </c>
-      <c r="L56" s="4">
-        <f>K56 - J56</f>
-        <v>1.6236212E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L56" s="20">
+        <f>I56 * 1000</f>
+        <v>17.540469999999999</v>
+      </c>
+      <c r="M56" s="20">
+        <f t="shared" si="25"/>
+        <v>11.209897999999999</v>
+      </c>
+      <c r="N56" s="20">
+        <f t="shared" si="26"/>
+        <v>27.446110000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>21</v>
       </c>
@@ -2273,9 +2470,17 @@
       <c r="K57" s="17">
         <v>2.7446109999999999E-2</v>
       </c>
-      <c r="L57" s="4">
-        <f>K57 - J57</f>
-        <v>1.6236212E-2</v>
+      <c r="L57" s="20">
+        <f>I57 * 1000</f>
+        <v>17.540469999999999</v>
+      </c>
+      <c r="M57" s="20">
+        <f t="shared" si="25"/>
+        <v>11.209897999999999</v>
+      </c>
+      <c r="N57" s="20">
+        <f t="shared" si="26"/>
+        <v>27.446110000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>